<commit_message>
fix excel AND statm bug, after Gavrilenko
</commit_message>
<xml_diff>
--- a/OSAT.xlsx
+++ b/OSAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/easonzz/Documents/GitHub/olspthermo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A099D1D4-586E-604E-BD13-EA2E9581039B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDB6E1B-673D-7F48-BC06-28056223C191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5160" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{F6D56C55-FC58-0A42-B3DC-AB43C104A521}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="27960" windowHeight="17500" xr2:uid="{F6D56C55-FC58-0A42-B3DC-AB43C104A521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,14 +363,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81FFB3C-A287-8841-85EE-7DDA979DC065}">
   <dimension ref="A1:BZ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="CB11" sqref="CB11"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BV12" sqref="BV12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,177 +746,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="6"/>
-      <c r="BK1" s="6"/>
-      <c r="BL1" s="6"/>
-      <c r="BM1" s="6"/>
-      <c r="BN1" s="6"/>
-      <c r="BO1" s="6"/>
-      <c r="BP1" s="6"/>
-      <c r="BQ1" s="6"/>
-      <c r="BR1" s="6"/>
-      <c r="BS1" s="6"/>
-      <c r="BT1" s="6"/>
-      <c r="BU1" s="6"/>
-      <c r="BV1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
+      <c r="BD1" s="7"/>
+      <c r="BE1" s="7"/>
+      <c r="BF1" s="7"/>
+      <c r="BG1" s="7"/>
+      <c r="BH1" s="7"/>
+      <c r="BI1" s="7"/>
+      <c r="BJ1" s="7"/>
+      <c r="BK1" s="7"/>
+      <c r="BL1" s="7"/>
+      <c r="BM1" s="7"/>
+      <c r="BN1" s="7"/>
+      <c r="BO1" s="7"/>
+      <c r="BP1" s="7"/>
+      <c r="BQ1" s="7"/>
+      <c r="BR1" s="7"/>
+      <c r="BS1" s="7"/>
+      <c r="BT1" s="7"/>
+      <c r="BU1" s="7"/>
+      <c r="BV1" s="7"/>
     </row>
     <row r="2" spans="1:78" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7" t="s">
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7" t="s">
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="7"/>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="7"/>
-      <c r="BD2" s="7"/>
-      <c r="BE2" s="7"/>
-      <c r="BF2" s="7"/>
-      <c r="BG2" s="7"/>
-      <c r="BH2" s="7"/>
-      <c r="BM2" s="8" t="s">
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BM2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="BN2" s="8"/>
-      <c r="BO2" s="8"/>
-      <c r="BP2" s="8"/>
-      <c r="BQ2" s="7" t="s">
+      <c r="BN2" s="6"/>
+      <c r="BO2" s="6"/>
+      <c r="BP2" s="6"/>
+      <c r="BQ2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="BR2" s="7"/>
-      <c r="BS2" s="8" t="s">
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="BT2" s="8"/>
-      <c r="BU2" s="8" t="s">
+      <c r="BT2" s="6"/>
+      <c r="BU2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="BV2" s="8"/>
-      <c r="BW2" s="8" t="s">
+      <c r="BV2" s="6"/>
+      <c r="BW2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="BX2" s="8"/>
-      <c r="BY2" s="8" t="s">
+      <c r="BX2" s="6"/>
+      <c r="BY2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="BZ2" s="8"/>
+      <c r="BZ2" s="6"/>
     </row>
     <row r="3" spans="1:78" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -1422,7 +1422,7 @@
         <v>5.1986355076170887E-2</v>
       </c>
       <c r="BU4" s="2">
-        <f>IF(AND(BM4&gt;BN4,BM4&gt;BO4),BM4,IF(BR4&gt;BQ4&gt;0.6744897*2,BO4,IF(BQ4&gt;BR4&gt;0.6744897*2,BN4,IF(AND(BQ4&lt;0.6744897*2,BR4&lt;0.6744897*2),BM4,IF(BR4&gt;0.6744897*2&gt;BQ4,BR4,IF(BQ4&gt;0.6744897*2&gt;BR4,BN4,BM4))))))</f>
+        <f>IF(AND(BM4&gt;BN4,BM4&gt;BO4),BM4,IF(AND(BR4&gt;BQ4, BQ4&gt;0.6744897*2),BO4,IF(AND(BQ4&gt;BR4, BR4&gt;0.6744897*2),BN4,IF(AND(BQ4&lt;0.6744897*2,BR4&lt;0.6744897*2),BM4,IF(AND(BR4&gt;0.6744897*2, 0.6744897*2&gt;BQ4),BO4,IF(AND(BQ4&gt;0.6744897*2, 0.6744897*2&gt;BR4),BN4,BM4))))))</f>
         <v>1171.2348235142249</v>
       </c>
       <c r="BV4" s="2">

</xml_diff>

<commit_message>
fix excel Fo calc bug, after Gavrilenko
</commit_message>
<xml_diff>
--- a/OSAT.xlsx
+++ b/OSAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/easonzz/Documents/GitHub/olspthermo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2CF533-BD39-444D-8915-5A5B87B76F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B60D73-4877-824D-BD03-3F8A2310ECF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="27960" windowHeight="17500" xr2:uid="{F6D56C55-FC58-0A42-B3DC-AB43C104A521}"/>
+    <workbookView xWindow="14820" yWindow="500" windowWidth="13980" windowHeight="17500" xr2:uid="{F6D56C55-FC58-0A42-B3DC-AB43C104A521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81FFB3C-A287-8841-85EE-7DDA979DC065}">
   <dimension ref="A1:BZ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BT12" sqref="BT12"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BD5" sqref="A5:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1386,7 +1386,7 @@
         <v>-6.5646415922300658</v>
       </c>
       <c r="BL4" s="2">
-        <f>H4/Sheet2!G2/(Sheet1!H4/Sheet2!G2+Sheet1!F4/Sheet2!E2)</f>
+        <f>H4/Sheet2!$G$2/(Sheet1!H4/Sheet2!$G$2+Sheet1!F4/Sheet2!$E$2)</f>
         <v>0.81907333876206956</v>
       </c>
       <c r="BM4" s="2">

</xml_diff>

<commit_message>
fix bugs: excel AND statm & Fo calc, after Gavrilenko
</commit_message>
<xml_diff>
--- a/OSAT.xlsx
+++ b/OSAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/easonzz/Documents/GitHub/olspthermo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B60D73-4877-824D-BD03-3F8A2310ECF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF634AFE-FB5E-D74E-ACCB-03FDD298A960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14820" yWindow="500" windowWidth="13980" windowHeight="17500" xr2:uid="{F6D56C55-FC58-0A42-B3DC-AB43C104A521}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t>sample_no</t>
   </si>
@@ -686,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81FFB3C-A287-8841-85EE-7DDA979DC065}">
-  <dimension ref="A1:BZ4"/>
+  <dimension ref="A1:BZ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
-      <selection activeCell="BD5" sqref="A5:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BJ7" sqref="BJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,6 +1446,298 @@
         <v>23.9</v>
       </c>
     </row>
+    <row r="5" spans="1:78" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>40.111999999999995</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.9200000000000002E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3.4100000000000005E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.6000000000000011E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>16.669000000000004</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.26899999999999996</v>
+      </c>
+      <c r="H5" s="2">
+        <v>42.334000000000003</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.24200000000000008</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="M5" s="2">
+        <v>99.905999999999992</v>
+      </c>
+      <c r="N5" s="2">
+        <v>7.1678571428571453E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2.3813809523809502</v>
+      </c>
+      <c r="P5" s="2">
+        <v>25.400154761904801</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>25.544071428571435</v>
+      </c>
+      <c r="R5" s="2">
+        <v>31.851000000000006</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0.25536904761904805</v>
+      </c>
+      <c r="T5" s="2">
+        <v>11.457654761904788</v>
+      </c>
+      <c r="U5" s="2">
+        <v>5.9404761904761896E-3</v>
+      </c>
+      <c r="V5" s="2">
+        <v>96.971690476190474</v>
+      </c>
+      <c r="W5" s="2">
+        <f>N5/Sheet2!A$2</f>
+        <v>1.1929667388747385E-3</v>
+      </c>
+      <c r="X5" s="2">
+        <f>O5/Sheet2!B$2</f>
+        <v>2.98172803926205E-2</v>
+      </c>
+      <c r="Y5" s="2">
+        <f>P5/Sheet2!C$2*2</f>
+        <v>0.49823140231993179</v>
+      </c>
+      <c r="Z5" s="2">
+        <f>Q5/Sheet2!D$2*2</f>
+        <v>0.33612743210849416</v>
+      </c>
+      <c r="AA5" s="2">
+        <f>R5/Sheet2!E$2</f>
+        <v>0.44333309207119842</v>
+      </c>
+      <c r="AB5" s="2">
+        <f>S5/Sheet2!F$2</f>
+        <v>3.5999186779193037E-3</v>
+      </c>
+      <c r="AC5" s="2">
+        <f>T5/Sheet2!G$2</f>
+        <v>0.28427801336590514</v>
+      </c>
+      <c r="AD5" s="2">
+        <f>SUM(X5:AC5)</f>
+        <v>1.5953871389360692</v>
+      </c>
+      <c r="AE5" s="2">
+        <f>2*(AB5+AC5)+3*(Z5+Y5)+4*X5</f>
+        <v>3.1981014889434092</v>
+      </c>
+      <c r="AF5" s="2">
+        <f>IF((AD5*8/3-AE5-2*AA5)&gt;0, AD5*8/3-AE5-2*AA5, 0)</f>
+        <v>0.16959803074371216</v>
+      </c>
+      <c r="AG5" s="2">
+        <f>AA5-AF5</f>
+        <v>0.27373506132748626</v>
+      </c>
+      <c r="AH5" s="2">
+        <f>IF(AG5&lt;0, AA5,AF5)</f>
+        <v>0.16959803074371216</v>
+      </c>
+      <c r="AI5" s="2">
+        <f>IF(AH5=0, ((1/3)*AD5+X5)/(AC5+AG5), 1)</f>
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="2">
+        <f>IF(AH5=0, (2/3)*AD5/(2*X5+Y5+Z5), 1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK5" s="2">
+        <f>(AG5+AB5+AC5)/(AB5+AC5+AG5)</f>
+        <v>1</v>
+      </c>
+      <c r="AL5" s="2">
+        <f>Z5*AJ5/2</f>
+        <v>0.16806371605424708</v>
+      </c>
+      <c r="AM5" s="2">
+        <f>(AG5*AI5+AB5*AI5-Z5*AJ5/2-AH5/2-2*X5*AJ5)*AK5</f>
+        <v>-3.5162312205938587E-2</v>
+      </c>
+      <c r="AN5" s="2">
+        <f>AH5/2</f>
+        <v>8.4799015371856079E-2</v>
+      </c>
+      <c r="AO5" s="2">
+        <f>AK5*AI5*AC5</f>
+        <v>0.28427801336590514</v>
+      </c>
+      <c r="AP5" s="2">
+        <f>AJ5*X5</f>
+        <v>2.98172803926205E-2</v>
+      </c>
+      <c r="AQ5" s="2">
+        <f>SUM(AL5:AP5)</f>
+        <v>0.53179571297869022</v>
+      </c>
+      <c r="AR5" s="2">
+        <f>AO5/AQ5</f>
+        <v>0.53456243897418654</v>
+      </c>
+      <c r="AS5" s="2">
+        <f>AL5/AQ5</f>
+        <v>0.31603059587090282</v>
+      </c>
+      <c r="AT5" s="2">
+        <f>AP5/AQ5</f>
+        <v>5.6069049947033552E-2</v>
+      </c>
+      <c r="AU5" s="2">
+        <f>AN5/AQ5</f>
+        <v>0.15945787696722952</v>
+      </c>
+      <c r="AV5" s="2">
+        <f>(1-AR5)*(1+AT5-AR5)</f>
+        <v>0.24272876507003963</v>
+      </c>
+      <c r="AW5" s="2">
+        <f>AS5*(1-AR5)</f>
+        <v>0.14709250975168753</v>
+      </c>
+      <c r="AX5" s="2">
+        <f>AT5*(1-AR5)</f>
+        <v>2.6096641856381813E-2</v>
+      </c>
+      <c r="AY5" s="2">
+        <f>AU5*(1-AR5)</f>
+        <v>7.4217685341981546E-2</v>
+      </c>
+      <c r="AZ5" s="2">
+        <f>AS5*(AS5+AT5+AU5)</f>
+        <v>0.16798844066545698</v>
+      </c>
+      <c r="BA5" s="2">
+        <f>AT5*(AS5+AT5+AU5)</f>
+        <v>2.980392529476289E-2</v>
+      </c>
+      <c r="BB5" s="2">
+        <f>AU5*(AS5+AT5+AU5)</f>
+        <v>8.4761034069282287E-2</v>
+      </c>
+      <c r="BC5" s="2">
+        <f>AS5*AT5</f>
+        <v>1.7719535264676425E-2</v>
+      </c>
+      <c r="BD5" s="2">
+        <f>AS5*AU5</f>
+        <v>5.0393567874262656E-2</v>
+      </c>
+      <c r="BE5" s="2">
+        <f>AT5*AU5</f>
+        <v>8.9406516681235226E-3</v>
+      </c>
+      <c r="BF5" s="2">
+        <f>AR5^0.5</f>
+        <v>0.73113777017343762</v>
+      </c>
+      <c r="BG5" s="2">
+        <f>AR5^2</f>
+        <v>0.2857570011620309</v>
+      </c>
+      <c r="BH5" s="2">
+        <f>AR5</f>
+        <v>0.53456243897418654</v>
+      </c>
+      <c r="BI5" s="2">
+        <f>Z5/(Z5+Y5)</f>
+        <v>0.40285716197726468</v>
+      </c>
+      <c r="BJ5" s="2">
+        <f>LN(D5/P5)</f>
+        <v>-6.6132131616869723</v>
+      </c>
+      <c r="BK5" s="2">
+        <f>LN(E5/Q5)</f>
+        <v>-6.5646415922300658</v>
+      </c>
+      <c r="BL5" s="2">
+        <f>H5/Sheet2!$G$2/(Sheet1!H5/Sheet2!$G$2+Sheet1!F5/Sheet2!$E$2)</f>
+        <v>0.81907333876206956</v>
+      </c>
+      <c r="BM5" s="2">
+        <f>10000/(-0.168118521 *(BJ5+0.654194424)/(0.390197643*AV5+0.00919774257*AW5-2.49266643*AX5+0.0646891489*AY5-0.0307131662*AZ5-4.14143648*BA5-0.427844629*BB5+4.63710203*BC5+0.054530766*BD5+10.8027441*BE5-0.630188015*BF5-0.593120349*BG5+1.4866989*BH5) + 2.7137923)-273.15</f>
+        <v>1090.821372580865</v>
+      </c>
+      <c r="BN5" s="2">
+        <f>10000/(0.0488-0.6572*BJ5-0.3886*BK5+0.5427*BI5)-273.15</f>
+        <v>1122.5908142538769</v>
+      </c>
+      <c r="BO5" s="2">
+        <f>10000/(0.7395-0.8654*BJ5+1.1438*BI5)-273.15</f>
+        <v>1171.2348235142249</v>
+      </c>
+      <c r="BP5" s="2">
+        <f>10000/(0.575+0.884*BI5-0.897*BJ5)-273.15</f>
+        <v>1183.9009596971014</v>
+      </c>
+      <c r="BQ5" s="2">
+        <f>ABS(BM5-BN5)/SQRT(23.9^2+34.2^2)</f>
+        <v>0.76142811124794862</v>
+      </c>
+      <c r="BR5" s="2">
+        <f>ABS(BM5-BO5)/SQRT(23.9^2+43.3^2)</f>
+        <v>1.6258916339460603</v>
+      </c>
+      <c r="BS5" s="2">
+        <f>1-_xlfn.NORM.DIST(BQ5, 0,1,TRUE)</f>
+        <v>0.22320070108369805</v>
+      </c>
+      <c r="BT5" s="2">
+        <f>1-_xlfn.NORM.DIST(BR5, 0,1,TRUE)</f>
+        <v>5.1986355076170887E-2</v>
+      </c>
+      <c r="BU5" s="2">
+        <f>IF(AND(BM5&gt;BN5,BM5&gt;BO5),BM5,IF(AND(BR5&gt;BQ5, BQ5&gt;0.6744897*2),BO5,IF(AND(BQ5&gt;BR5, BR5&gt;0.6744897*2),BN5,IF(AND(BQ5&lt;0.6744897*2,BR5&lt;0.6744897*2),BM5,IF(AND(BR5&gt;0.6744897*2, 0.6744897*2&gt;BQ5),BO5,IF(AND(BQ5&gt;0.6744897*2, 0.6744897*2&gt;BR5),BN5,BM5))))))</f>
+        <v>1171.2348235142249</v>
+      </c>
+      <c r="BV5" s="2">
+        <f>IF(BU5=BN5,34.2,IF(BU5=BM5,23.9,IF(BU5=BO5,43.4)))</f>
+        <v>43.4</v>
+      </c>
+      <c r="BW5" s="2">
+        <f>IF(BR5&gt; 0.6744897 *2, BO5,BM5)</f>
+        <v>1171.2348235142249</v>
+      </c>
+      <c r="BX5" s="2">
+        <f>IF(BW5=BO5, 43.3, 23.9)</f>
+        <v>43.3</v>
+      </c>
+      <c r="BY5" s="2">
+        <f>IF(BQ5&gt;0.6744897*2, BN5, BM5)</f>
+        <v>1090.821372580865</v>
+      </c>
+      <c r="BZ5" s="2">
+        <f>IF(BY5=BN5,34.2,23.9)</f>
+        <v>23.9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="BW2:BX2"/>

</xml_diff>